<commit_message>
Add last version to git
</commit_message>
<xml_diff>
--- a/Lower1.xlsx
+++ b/Lower1.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,488 +458,2054 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44867.75</v>
+        <v>44089.61458333334</v>
       </c>
       <c r="B2" t="n">
-        <v>20170.34201374912</v>
+        <v>2.997434750768776</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44867.76041666666</v>
+        <v>44090.66666666666</v>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>20457.81431486085</v>
+        <v>2.626344181182382</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44867.80208333334</v>
+        <v>44094.54166666666</v>
       </c>
       <c r="B4" t="n">
-        <v>20074.44932023154</v>
+        <v>2.775149481780416</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44868.0625</v>
+        <v>44094.96875</v>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>20292.0083434662</v>
+        <v>2.817188273603734</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44871.96875</v>
+        <v>44095.4375</v>
       </c>
       <c r="B6" t="n">
-        <v>20976.596386877</v>
+        <v>2.58082824307663</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44872.66666666666</v>
+        <v>44095.6875</v>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>20774.0707720491</v>
+        <v>2.699081890485809</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44872.92708333334</v>
+        <v>44102.98958333334</v>
       </c>
       <c r="B8" t="n">
-        <v>20436.66941051499</v>
+        <v>2.91253062481028</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44873.09375</v>
+        <v>44103.28125</v>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
-        <v>20672.14488114764</v>
+        <v>2.969744725475934</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44873.13541666666</v>
+        <v>44104.5</v>
       </c>
       <c r="B10" t="n">
-        <v>20315.98471242522</v>
+        <v>2.832966261823647</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44873.66666666666</v>
+        <v>44104.66666666666</v>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>19746.93872516882</v>
+        <v>2.905301245201406</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44873.75</v>
+        <v>44105.65625</v>
       </c>
       <c r="B12" t="n">
-        <v>19000.86603372202</v>
+        <v>2.869455588481171</v>
       </c>
       <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44875.13541666666</v>
+        <v>44105.6875</v>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>16486.65264751405</v>
+        <v>2.930716418560302</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44876.59375</v>
+        <v>44105.77083333334</v>
       </c>
       <c r="B14" t="n">
-        <v>16458.80126784409</v>
+        <v>2.781898584636382</v>
       </c>
       <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44876.61458333334</v>
+        <v>44105.9375</v>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="n">
-        <v>17253.94750620751</v>
+        <v>2.830988566391733</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44878.375</v>
+        <v>44106.3125</v>
       </c>
       <c r="B16" t="n">
-        <v>16476.65378640195</v>
+        <v>2.666263870707016</v>
       </c>
       <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44878.58333333334</v>
+        <v>44106.58333333334</v>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
-        <v>16712.50775876605</v>
+        <v>2.630449014213091</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44878.875</v>
+        <v>44107.91666666666</v>
       </c>
       <c r="B18" t="n">
-        <v>16250.04212720195</v>
+        <v>2.552326850638778</v>
       </c>
       <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44879.27083333334</v>
+        <v>44108.3125</v>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="n">
-        <v>16230.22009422589</v>
+        <v>2.548202028840201</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44885.47916666666</v>
+        <v>44108.66666666666</v>
       </c>
       <c r="B20" t="n">
-        <v>16511.52594678809</v>
+        <v>2.436413467691166</v>
       </c>
       <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44885.63541666666</v>
+        <v>44108.83333333334</v>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="n">
-        <v>16620.79388291823</v>
+        <v>2.500112939553169</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44885.92708333334</v>
+        <v>44110.32291666666</v>
       </c>
       <c r="B22" t="n">
-        <v>16330.55249788763</v>
+        <v>2.523090878807674</v>
       </c>
       <c r="C22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44886.17708333334</v>
+        <v>44111.21875</v>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="n">
-        <v>16318.36677990177</v>
+        <v>2.221048679547392</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44886.82291666666</v>
+        <v>44112.23958333334</v>
       </c>
       <c r="B24" t="n">
-        <v>15685.85565439299</v>
+        <v>2.131799553958633</v>
       </c>
       <c r="C24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44887.01041666666</v>
+        <v>44112.42708333334</v>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
-        <v>15935.60787453595</v>
+        <v>2.182479925400636</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44892.97916666666</v>
+        <v>44117.125</v>
       </c>
       <c r="B26" t="n">
-        <v>16407.95206639424</v>
+        <v>2.454595875516119</v>
       </c>
       <c r="C26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44893.52083333334</v>
+        <v>44117.34375</v>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="n">
-        <v>16235.99732739341</v>
+        <v>2.530948096025645</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44900.63541666666</v>
+        <v>44117.73958333334</v>
       </c>
       <c r="B28" t="n">
-        <v>17048.48863740604</v>
+        <v>2.339580924900689</v>
       </c>
       <c r="C28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44901.02083333334</v>
+        <v>44117.875</v>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="n">
-        <v>17047.30387308295</v>
+        <v>2.427303578820448</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44902.34375</v>
+        <v>44118.65625</v>
       </c>
       <c r="B30" t="n">
-        <v>16782.94895432819</v>
+        <v>2.269193507595558</v>
       </c>
       <c r="C30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44902.60416666666</v>
+        <v>44118.95833333334</v>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="n">
-        <v>16880.48499607055</v>
+        <v>2.298694976328575</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44907.17708333334</v>
+        <v>44120.16666666666</v>
       </c>
       <c r="B32" t="n">
-        <v>16917.67953154405</v>
+        <v>2.182458999422909</v>
       </c>
       <c r="C32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44907.40625</v>
+        <v>44120.48958333334</v>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="n">
-        <v>16972.9260362305</v>
+        <v>2.191469830027393</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44910.69791666666</v>
+        <v>44123.03125</v>
       </c>
       <c r="B34" t="n">
-        <v>17341.95720423076</v>
+        <v>2.1603393197545</v>
       </c>
       <c r="C34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44911.10416666666</v>
+        <v>44123.54166666666</v>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="n">
-        <v>17419.66749216793</v>
+        <v>2.107727062128928</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44911.36458333334</v>
+        <v>44124.32291666666</v>
       </c>
       <c r="B36" t="n">
-        <v>17196.87230702792</v>
+        <v>2.002046365479273</v>
       </c>
       <c r="C36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44912.27083333334</v>
+        <v>44124.84375</v>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="n">
-        <v>16738.18114085326</v>
+        <v>1.915600803314232</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44914.72916666666</v>
+        <v>44126.96875</v>
       </c>
       <c r="B38" t="n">
-        <v>16534.4787757376</v>
+        <v>1.943049241158885</v>
       </c>
       <c r="C38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44915.0625</v>
+        <v>44127.20833333334</v>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="n">
-        <v>16570.5964488361</v>
+        <v>1.981254652117348</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44917.60416666666</v>
+        <v>44129.23958333334</v>
       </c>
       <c r="B40" t="n">
-        <v>16676.97660180337</v>
+        <v>1.858307958759255</v>
       </c>
       <c r="C40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44917.84375</v>
+        <v>44129.59375</v>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="n">
-        <v>16722.45074095321</v>
+        <v>1.889557201885713</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44920.60416666666</v>
+        <v>44129.66666666666</v>
       </c>
       <c r="B42" t="n">
-        <v>16760.63784807087</v>
+        <v>1.82189517075862</v>
       </c>
       <c r="C42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>44920.61458333334</v>
+        <v>44130.08333333334</v>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="n">
-        <v>16823.80216547004</v>
+        <v>1.82061155675064</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>44920.79166666666</v>
+        <v>44130.77083333334</v>
       </c>
       <c r="B44" t="n">
-        <v>16729.25621113323</v>
+        <v>1.698728763958088</v>
       </c>
       <c r="C44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>44920.88541666666</v>
+        <v>44131.08333333334</v>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="n">
-        <v>16802.31749870565</v>
+        <v>1.708347335846987</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>44922.60416666666</v>
+        <v>44131.33333333334</v>
       </c>
       <c r="B46" t="n">
-        <v>16748.82374725206</v>
+        <v>1.60702833527638</v>
       </c>
       <c r="C46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>44923.05208333334</v>
+        <v>44131.42708333334</v>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="n">
-        <v>16723.63397160145</v>
+        <v>1.673266774810412</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>44923.125</v>
+        <v>44132.1875</v>
       </c>
       <c r="B48" t="n">
-        <v>16569.7416409459</v>
+        <v>1.59223154384136</v>
       </c>
       <c r="C48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>44923.40625</v>
+        <v>44132.52083333334</v>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="n">
-        <v>16662.38208704476</v>
+        <v>1.599063398662677</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>44923.88541666666</v>
+        <v>44133.51041666666</v>
       </c>
       <c r="B50" t="n">
-        <v>16484.90191279291</v>
+        <v>1.457359343173884</v>
       </c>
       <c r="C50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>44924.17708333334</v>
+        <v>44133.58333333334</v>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="n">
-        <v>16572.65073458746</v>
+        <v>1.523473848442751</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>44925.3125</v>
+        <v>44133.94791666666</v>
       </c>
       <c r="B52" t="n">
-        <v>16468.53259765337</v>
+        <v>1.418255785735927</v>
       </c>
       <c r="C52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>44925.63541666666</v>
+        <v>44134.51041666666</v>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="n">
-        <v>16517.11042651413</v>
+        <v>1.390418110229577</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>44926.94791666666</v>
+        <v>44137.35416666666</v>
       </c>
       <c r="B54" t="n">
-        <v>16476.73232444436</v>
+        <v>1.545933786218812</v>
       </c>
       <c r="C54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>44927.10416666666</v>
+        <v>44137.90625</v>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="n">
-        <v>16559.60673459858</v>
+        <v>1.491771848317311</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>44138.125</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.431950367436246</v>
+      </c>
+      <c r="C56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>44138.34375</v>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="n">
+        <v>1.460928167639542</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>44139.03125</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1.382073616027115</v>
+      </c>
+      <c r="C58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>44139.41666666666</v>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="n">
+        <v>1.375994068739984</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>44139.59375</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1.308547706069045</v>
+      </c>
+      <c r="C60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>44139.67708333334</v>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="n">
+        <v>1.351471627836466</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>44140.46875</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1.342706622224052</v>
+      </c>
+      <c r="C62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>44140.58333333334</v>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="n">
+        <v>1.370658300155706</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>44146.8125</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2.020106055715557</v>
+      </c>
+      <c r="C64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>44147.11458333334</v>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="n">
+        <v>2.048623100131806</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>44147.67708333334</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.882620678174391</v>
+      </c>
+      <c r="C66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>44147.97916666666</v>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="n">
+        <v>1.90021801282828</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>44150.91666666666</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.949036743171241</v>
+      </c>
+      <c r="C68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>44151.04166666666</v>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="n">
+        <v>2.065407583821417</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>44153.23958333334</v>
+      </c>
+      <c r="B70" t="n">
+        <v>2.054630464404142</v>
+      </c>
+      <c r="C70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>44153.69791666666</v>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="n">
+        <v>2.087927372590663</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>44161.09375</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2.11384556857856</v>
+      </c>
+      <c r="C72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>44161.85416666666</v>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="n">
+        <v>1.819467800485715</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>44169.14583333334</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2.018430134694583</v>
+      </c>
+      <c r="C74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>44169.35416666666</v>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="n">
+        <v>2.07155880752894</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>44169.42708333334</v>
+      </c>
+      <c r="B76" t="n">
+        <v>1.981201949492947</v>
+      </c>
+      <c r="C76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>44170.27083333334</v>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="n">
+        <v>1.88596258648375</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>44171.38541666666</v>
+      </c>
+      <c r="B78" t="n">
+        <v>1.873449122165597</v>
+      </c>
+      <c r="C78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>44171.85416666666</v>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="n">
+        <v>1.857474917642344</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>44173.13541666666</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1.789001501702587</v>
+      </c>
+      <c r="C80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>44173.67708333334</v>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="n">
+        <v>1.731193274007974</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>44173.95833333334</v>
+      </c>
+      <c r="B82" t="n">
+        <v>1.631966186723473</v>
+      </c>
+      <c r="C82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>44174.48958333334</v>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="n">
+        <v>1.622281584551328</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>44176.07291666666</v>
+      </c>
+      <c r="B84" t="n">
+        <v>1.505109236791222</v>
+      </c>
+      <c r="C84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>44176.58333333334</v>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="n">
+        <v>1.489811264663942</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>44181.13541666666</v>
+      </c>
+      <c r="B86" t="n">
+        <v>1.600691999020268</v>
+      </c>
+      <c r="C86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>44181.26041666666</v>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="n">
+        <v>1.678760562052345</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>44185.01041666666</v>
+      </c>
+      <c r="B88" t="n">
+        <v>1.638272589568011</v>
+      </c>
+      <c r="C88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>44185.27083333334</v>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="n">
+        <v>1.660231142569955</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>44185.79166666666</v>
+      </c>
+      <c r="B90" t="n">
+        <v>1.592244679824349</v>
+      </c>
+      <c r="C90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="n">
+        <v>44186.07291666666</v>
+      </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="n">
+        <v>1.595449927742316</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="n">
+        <v>44186.42708333334</v>
+      </c>
+      <c r="B92" t="n">
+        <v>1.515145662855855</v>
+      </c>
+      <c r="C92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>44186.77083333334</v>
+      </c>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="n">
+        <v>1.542124450767078</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="n">
+        <v>44188.21875</v>
+      </c>
+      <c r="B94" t="n">
+        <v>1.425044132954645</v>
+      </c>
+      <c r="C94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>44189.0625</v>
+      </c>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="n">
+        <v>1.265586180957891</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>44191.4375</v>
+      </c>
+      <c r="B96" t="n">
+        <v>1.348980677933807</v>
+      </c>
+      <c r="C96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>44191.67708333334</v>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="n">
+        <v>1.374895633783284</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>44196.54166666666</v>
+      </c>
+      <c r="B98" t="n">
+        <v>1.413166624254213</v>
+      </c>
+      <c r="C98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>44196.67708333334</v>
+      </c>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="n">
+        <v>1.48315925569201</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>44202.82291666666</v>
+      </c>
+      <c r="B100" t="n">
+        <v>1.735553472495887</v>
+      </c>
+      <c r="C100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>44202.96875</v>
+      </c>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="n">
+        <v>1.925274712335233</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>44207.29166666666</v>
+      </c>
+      <c r="B102" t="n">
+        <v>2.911132626340587</v>
+      </c>
+      <c r="C102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>44207.85416666666</v>
+      </c>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="n">
+        <v>2.884944983454965</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="n">
+        <v>44211.65625</v>
+      </c>
+      <c r="B104" t="n">
+        <v>3.121865047570658</v>
+      </c>
+      <c r="C104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>44211.9375</v>
+      </c>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="n">
+        <v>3.230715607712678</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>44212.48958333334</v>
+      </c>
+      <c r="B106" t="n">
+        <v>3.204442547006365</v>
+      </c>
+      <c r="C106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>44212.5</v>
+      </c>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="n">
+        <v>3.425210785599247</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>44215.8125</v>
+      </c>
+      <c r="B108" t="n">
+        <v>3.611218141446532</v>
+      </c>
+      <c r="C108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>44216.57291666666</v>
+      </c>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="n">
+        <v>3.541440142950498</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>44217.91666666666</v>
+      </c>
+      <c r="B110" t="n">
+        <v>3.109968251351075</v>
+      </c>
+      <c r="C110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>44218.15625</v>
+      </c>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="n">
+        <v>3.101020120276233</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
+        <v>44225.25</v>
+      </c>
+      <c r="B112" t="n">
+        <v>3.652090614763016</v>
+      </c>
+      <c r="C112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>44225.47916666666</v>
+      </c>
+      <c r="B113" t="inlineStr"/>
+      <c r="C113" t="n">
+        <v>3.74590115714166</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>44233.19791666666</v>
+      </c>
+      <c r="B114" t="n">
+        <v>6.084461649971043</v>
+      </c>
+      <c r="C114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>44233.73958333334</v>
+      </c>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="n">
+        <v>6.022875422410603</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>44240.45833333334</v>
+      </c>
+      <c r="B116" t="n">
+        <v>8.827352855910572</v>
+      </c>
+      <c r="C116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>44240.625</v>
+      </c>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="n">
+        <v>9.165530330019473</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>44242.15625</v>
+      </c>
+      <c r="B118" t="n">
+        <v>8.131829076943761</v>
+      </c>
+      <c r="C118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>44242.35416666666</v>
+      </c>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="n">
+        <v>8.369873372139002</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>44243.67708333334</v>
+      </c>
+      <c r="B120" t="n">
+        <v>8.218945261380176</v>
+      </c>
+      <c r="C120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>44244</v>
+      </c>
+      <c r="B121" t="inlineStr"/>
+      <c r="C121" t="n">
+        <v>8.313912680974212</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>44244.15625</v>
+      </c>
+      <c r="B122" t="n">
+        <v>7.754964180304319</v>
+      </c>
+      <c r="C122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>44244.32291666666</v>
+      </c>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" t="n">
+        <v>7.966585867128075</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>44246.08333333334</v>
+      </c>
+      <c r="B124" t="n">
+        <v>8.561547073017071</v>
+      </c>
+      <c r="C124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>44246.26041666666</v>
+      </c>
+      <c r="B125" t="inlineStr"/>
+      <c r="C125" t="n">
+        <v>8.867261925088236</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>44247.9375</v>
+      </c>
+      <c r="B126" t="n">
+        <v>9.919683621314578</v>
+      </c>
+      <c r="C126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>44248.08333333334</v>
+      </c>
+      <c r="B127" t="inlineStr"/>
+      <c r="C127" t="n">
+        <v>10.37062517488999</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
+        <v>44249.42708333334</v>
+      </c>
+      <c r="B128" t="n">
+        <v>9.989542179466007</v>
+      </c>
+      <c r="C128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>44249.61458333334</v>
+      </c>
+      <c r="B129" t="inlineStr"/>
+      <c r="C129" t="n">
+        <v>10.28836147115143</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>44252.90625</v>
+      </c>
+      <c r="B130" t="n">
+        <v>14.52263445131015</v>
+      </c>
+      <c r="C130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
+        <v>44253.44791666666</v>
+      </c>
+      <c r="B131" t="inlineStr"/>
+      <c r="C131" t="n">
+        <v>13.99386036117554</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="n">
+        <v>44255.08333333334</v>
+      </c>
+      <c r="B132" t="n">
+        <v>12.61490154584406</v>
+      </c>
+      <c r="C132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="n">
+        <v>44255.77083333334</v>
+      </c>
+      <c r="B133" t="inlineStr"/>
+      <c r="C133" t="n">
+        <v>12.06594024763176</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>44257.79166666666</v>
+      </c>
+      <c r="B134" t="n">
+        <v>13.7762339051225</v>
+      </c>
+      <c r="C134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>44258.07291666666</v>
+      </c>
+      <c r="B135" t="inlineStr"/>
+      <c r="C135" t="n">
+        <v>14.08217166387515</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>44259.78125</v>
+      </c>
+      <c r="B136" t="n">
+        <v>12.8527175834854</v>
+      </c>
+      <c r="C136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>44260.47916666666</v>
+      </c>
+      <c r="B137" t="inlineStr"/>
+      <c r="C137" t="n">
+        <v>12.49886472851452</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>44266.03125</v>
+      </c>
+      <c r="B138" t="n">
+        <v>13.94871377391865</v>
+      </c>
+      <c r="C138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>44266.44791666666</v>
+      </c>
+      <c r="B139" t="inlineStr"/>
+      <c r="C139" t="n">
+        <v>14.0461752721206</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="n">
+        <v>44267.54166666666</v>
+      </c>
+      <c r="B140" t="n">
+        <v>15.09465829138884</v>
+      </c>
+      <c r="C140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>44268.21875</v>
+      </c>
+      <c r="B141" t="inlineStr"/>
+      <c r="C141" t="n">
+        <v>14.49075860085157</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>44270.3125</v>
+      </c>
+      <c r="B142" t="n">
+        <v>13.91817947689698</v>
+      </c>
+      <c r="C142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>44270.44791666666</v>
+      </c>
+      <c r="B143" t="inlineStr"/>
+      <c r="C143" t="n">
+        <v>14.30808121364502</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
+        <v>44271.22916666666</v>
+      </c>
+      <c r="B144" t="n">
+        <v>13.34688943993787</v>
+      </c>
+      <c r="C144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="n">
+        <v>44271.39583333334</v>
+      </c>
+      <c r="B145" t="inlineStr"/>
+      <c r="C145" t="n">
+        <v>13.75654234282177</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="n">
+        <v>44272.40625</v>
+      </c>
+      <c r="B146" t="n">
+        <v>13.09897465331895</v>
+      </c>
+      <c r="C146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="n">
+        <v>44272.55208333334</v>
+      </c>
+      <c r="B147" t="inlineStr"/>
+      <c r="C147" t="n">
+        <v>13.46133392666388</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>44276</v>
+      </c>
+      <c r="B148" t="n">
+        <v>14.12920261087028</v>
+      </c>
+      <c r="C148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>44276.58333333334</v>
+      </c>
+      <c r="B149" t="inlineStr"/>
+      <c r="C149" t="n">
+        <v>13.9278450504785</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>44277.91666666666</v>
+      </c>
+      <c r="B150" t="n">
+        <v>14.84414693903963</v>
+      </c>
+      <c r="C150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="n">
+        <v>44278.51041666666</v>
+      </c>
+      <c r="B151" t="inlineStr"/>
+      <c r="C151" t="n">
+        <v>14.63290352321864</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>44279.97916666666</v>
+      </c>
+      <c r="B152" t="n">
+        <v>13.90923599377436</v>
+      </c>
+      <c r="C152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>44280.77083333334</v>
+      </c>
+      <c r="B153" t="inlineStr"/>
+      <c r="C153" t="n">
+        <v>13.08219313372434</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="n">
+        <v>44286.14583333334</v>
+      </c>
+      <c r="B154" t="n">
+        <v>18.28460705931915</v>
+      </c>
+      <c r="C154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="2" t="n">
+        <v>44286.28125</v>
+      </c>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="n">
+        <v>19.06916011350191</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="n">
+        <v>44286.33333333334</v>
+      </c>
+      <c r="B156" t="n">
+        <v>18.04155168495493</v>
+      </c>
+      <c r="C156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="n">
+        <v>44286.41666666666</v>
+      </c>
+      <c r="B157" t="inlineStr"/>
+      <c r="C157" t="n">
+        <v>18.92073037968918</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>44296.86458333334</v>
+      </c>
+      <c r="B158" t="n">
+        <v>26.01965762208291</v>
+      </c>
+      <c r="C158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="n">
+        <v>44297.32291666666</v>
+      </c>
+      <c r="B159" t="inlineStr"/>
+      <c r="C159" t="n">
+        <v>26.43498829876617</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="n">
+        <v>44298.625</v>
+      </c>
+      <c r="B160" t="n">
+        <v>26.85671756898546</v>
+      </c>
+      <c r="C160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>44298.84375</v>
+      </c>
+      <c r="B161" t="inlineStr"/>
+      <c r="C161" t="n">
+        <v>27.81974798013037</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>44299.30208333334</v>
+      </c>
+      <c r="B162" t="n">
+        <v>26.67625913699258</v>
+      </c>
+      <c r="C162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>44299.59375</v>
+      </c>
+      <c r="B163" t="inlineStr"/>
+      <c r="C163" t="n">
+        <v>27.28592745049205</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>44300.38541666666</v>
+      </c>
+      <c r="B164" t="n">
+        <v>25.58677973286655</v>
+      </c>
+      <c r="C164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="n">
+        <v>44300.6875</v>
+      </c>
+      <c r="B165" t="inlineStr"/>
+      <c r="C165" t="n">
+        <v>26.17391081983996</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>44302.44791666666</v>
+      </c>
+      <c r="B166" t="n">
+        <v>25.81413991024876</v>
+      </c>
+      <c r="C166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>44302.80208333334</v>
+      </c>
+      <c r="B167" t="inlineStr"/>
+      <c r="C167" t="n">
+        <v>26.09829203646458</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="n">
+        <v>44304.01041666666</v>
+      </c>
+      <c r="B168" t="n">
+        <v>24.46239588744731</v>
+      </c>
+      <c r="C168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>44304.14583333334</v>
+      </c>
+      <c r="B169" t="inlineStr"/>
+      <c r="C169" t="n">
+        <v>24.71424434749494</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>44319.84375</v>
+      </c>
+      <c r="B170" t="n">
+        <v>45.42712652291905</v>
+      </c>
+      <c r="C170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="n">
+        <v>44320.20833333334</v>
+      </c>
+      <c r="B171" t="inlineStr"/>
+      <c r="C171" t="n">
+        <v>45.884710454005</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="n">
+        <v>44320.69791666666</v>
+      </c>
+      <c r="B172" t="n">
+        <v>42.55398989152982</v>
+      </c>
+      <c r="C172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="2" t="n">
+        <v>44321.04166666666</v>
+      </c>
+      <c r="B173" t="inlineStr"/>
+      <c r="C173" t="n">
+        <v>44.32897495479471</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="n">
+        <v>44326.84375</v>
+      </c>
+      <c r="B174" t="n">
+        <v>41.3860616919868</v>
+      </c>
+      <c r="C174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>44326.90625</v>
+      </c>
+      <c r="B175" t="inlineStr"/>
+      <c r="C175" t="n">
+        <v>43.53030316279118</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>44335.46875</v>
+      </c>
+      <c r="B176" t="n">
+        <v>43.16489576269026</v>
+      </c>
+      <c r="C176" t="inlineStr"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="n">
+        <v>44335.63541666666</v>
+      </c>
+      <c r="B177" t="inlineStr"/>
+      <c r="C177" t="n">
+        <v>45.68648690290231</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="n">
+        <v>44337.59375</v>
+      </c>
+      <c r="B178" t="n">
+        <v>36.9388997954529</v>
+      </c>
+      <c r="C178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>44337.98958333334</v>
+      </c>
+      <c r="B179" t="inlineStr"/>
+      <c r="C179" t="n">
+        <v>38.88827146100983</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="n">
+        <v>44339.32291666666</v>
+      </c>
+      <c r="B180" t="n">
+        <v>26.37381015181172</v>
+      </c>
+      <c r="C180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="n">
+        <v>44339.83333333334</v>
+      </c>
+      <c r="B181" t="inlineStr"/>
+      <c r="C181" t="n">
+        <v>23.61274779655797</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="n">
+        <v>44344.23958333334</v>
+      </c>
+      <c r="B182" t="n">
+        <v>31.06890134617295</v>
+      </c>
+      <c r="C182" t="inlineStr"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="2" t="n">
+        <v>44344.54166666666</v>
+      </c>
+      <c r="B183" t="inlineStr"/>
+      <c r="C183" t="n">
+        <v>31.18346857858034</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="n">
+        <v>44351.30208333334</v>
+      </c>
+      <c r="B184" t="n">
+        <v>34.94115467540419</v>
+      </c>
+      <c r="C184" t="inlineStr"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="2" t="n">
+        <v>44351.53125</v>
+      </c>
+      <c r="B185" t="inlineStr"/>
+      <c r="C185" t="n">
+        <v>37.16245947376434</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="n">
+        <v>44354.875</v>
+      </c>
+      <c r="B186" t="n">
+        <v>39.82638702879124</v>
+      </c>
+      <c r="C186" t="inlineStr"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="n">
+        <v>44355.35416666666</v>
+      </c>
+      <c r="B187" t="inlineStr"/>
+      <c r="C187" t="n">
+        <v>38.11796616795971</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="n">
+        <v>44358.89583333334</v>
+      </c>
+      <c r="B188" t="n">
+        <v>35.70436854395756</v>
+      </c>
+      <c r="C188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="n">
+        <v>44359.16666666666</v>
+      </c>
+      <c r="B189" t="inlineStr"/>
+      <c r="C189" t="n">
+        <v>36.31918575230875</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="2" t="n">
+        <v>44365.55208333334</v>
+      </c>
+      <c r="B190" t="n">
+        <v>36.89115262643637</v>
+      </c>
+      <c r="C190" t="inlineStr"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="2" t="n">
+        <v>44365.875</v>
+      </c>
+      <c r="B191" t="inlineStr"/>
+      <c r="C191" t="n">
+        <v>36.77809900867496</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="2" t="n">
+        <v>44367.41666666666</v>
+      </c>
+      <c r="B192" t="n">
+        <v>33.46723335148908</v>
+      </c>
+      <c r="C192" t="inlineStr"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="2" t="n">
+        <v>44367.63541666666</v>
+      </c>
+      <c r="B193" t="inlineStr"/>
+      <c r="C193" t="n">
+        <v>33.99281598173719</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="2" t="n">
+        <v>44368.27083333334</v>
+      </c>
+      <c r="B194" t="n">
+        <v>31.0902529912982</v>
+      </c>
+      <c r="C194" t="inlineStr"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="n">
+        <v>44368.58333333334</v>
+      </c>
+      <c r="B195" t="inlineStr"/>
+      <c r="C195" t="n">
+        <v>31.38261445987327</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="2" t="n">
+        <v>44369.48958333334</v>
+      </c>
+      <c r="B196" t="n">
+        <v>22.18599474278348</v>
+      </c>
+      <c r="C196" t="inlineStr"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="2" t="n">
+        <v>44369.61458333334</v>
+      </c>
+      <c r="B197" t="inlineStr"/>
+      <c r="C197" t="n">
+        <v>24.53420102432223</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="2" t="n">
+        <v>44377.15625</v>
+      </c>
+      <c r="B198" t="n">
+        <v>32.24151679526272</v>
+      </c>
+      <c r="C198" t="inlineStr"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="2" t="n">
+        <v>44377.32291666666</v>
+      </c>
+      <c r="B199" t="inlineStr"/>
+      <c r="C199" t="n">
+        <v>33.44275241315538</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="2" t="n">
+        <v>44382.16666666666</v>
+      </c>
+      <c r="B200" t="n">
+        <v>33.27284557526883</v>
+      </c>
+      <c r="C200" t="inlineStr"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="2" t="n">
+        <v>44382.41666666666</v>
+      </c>
+      <c r="B201" t="inlineStr"/>
+      <c r="C201" t="n">
+        <v>34.0693964613146</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="2" t="n">
+        <v>44385.3125</v>
+      </c>
+      <c r="B202" t="n">
+        <v>34.04155109914555</v>
+      </c>
+      <c r="C202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="2" t="n">
+        <v>44386.13541666666</v>
+      </c>
+      <c r="B203" t="inlineStr"/>
+      <c r="C203" t="n">
+        <v>33.36173792842835</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="2" t="n">
+        <v>44387.83333333334</v>
+      </c>
+      <c r="B204" t="n">
+        <v>31.08090429134454</v>
+      </c>
+      <c r="C204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="2" t="n">
+        <v>44388.0625</v>
+      </c>
+      <c r="B205" t="inlineStr"/>
+      <c r="C205" t="n">
+        <v>32.01146871920783</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="2" t="n">
+        <v>44389.41666666666</v>
+      </c>
+      <c r="B206" t="n">
+        <v>31.30772898621853</v>
+      </c>
+      <c r="C206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="2" t="n">
+        <v>44389.92708333334</v>
+      </c>
+      <c r="B207" t="inlineStr"/>
+      <c r="C207" t="n">
+        <v>30.91618151381613</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="2" t="n">
+        <v>44390.52083333334</v>
+      </c>
+      <c r="B208" t="n">
+        <v>29.39615985848453</v>
+      </c>
+      <c r="C208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="2" t="n">
+        <v>44390.64583333334</v>
+      </c>
+      <c r="B209" t="inlineStr"/>
+      <c r="C209" t="n">
+        <v>30.17425696984529</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="2" t="n">
+        <v>44391.04166666666</v>
+      </c>
+      <c r="B210" t="n">
+        <v>28.26875643133596</v>
+      </c>
+      <c r="C210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="2" t="n">
+        <v>44391.375</v>
+      </c>
+      <c r="B211" t="inlineStr"/>
+      <c r="C211" t="n">
+        <v>28.45383817670718</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="2" t="n">
+        <v>44393.42708333334</v>
+      </c>
+      <c r="B212" t="n">
+        <v>27.03802922216585</v>
+      </c>
+      <c r="C212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="2" t="n">
+        <v>44393.53125</v>
+      </c>
+      <c r="B213" t="inlineStr"/>
+      <c r="C213" t="n">
+        <v>28.16693394027036</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="2" t="n">
+        <v>44396.51041666666</v>
+      </c>
+      <c r="B214" t="n">
+        <v>24.65897354379702</v>
+      </c>
+      <c r="C214" t="inlineStr"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="2" t="n">
+        <v>44396.88541666666</v>
+      </c>
+      <c r="B215" t="inlineStr"/>
+      <c r="C215" t="n">
+        <v>24.58537442814149</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="2" t="n">
+        <v>44397.16666666666</v>
+      </c>
+      <c r="B216" t="n">
+        <v>22.84477885533662</v>
+      </c>
+      <c r="C216" t="inlineStr"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="2" t="n">
+        <v>44397.5</v>
+      </c>
+      <c r="B217" t="inlineStr"/>
+      <c r="C217" t="n">
+        <v>23.11434824609894</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="2" t="n">
+        <v>44402.57291666666</v>
+      </c>
+      <c r="B218" t="n">
+        <v>26.80055753393773</v>
+      </c>
+      <c r="C218" t="inlineStr"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="2" t="n">
+        <v>44402.77083333334</v>
+      </c>
+      <c r="B219" t="inlineStr"/>
+      <c r="C219" t="n">
+        <v>27.68547036117966</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="2" t="n">
+        <v>44409.96875</v>
+      </c>
+      <c r="B220" t="n">
+        <v>33.25372766317948</v>
+      </c>
+      <c r="C220" t="inlineStr"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="2" t="n">
+        <v>44410.11458333334</v>
+      </c>
+      <c r="B221" t="inlineStr"/>
+      <c r="C221" t="n">
+        <v>34.77371320359708</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="2" t="n">
+        <v>44415.67708333334</v>
+      </c>
+      <c r="B222" t="n">
+        <v>37.62421031695892</v>
+      </c>
+      <c r="C222" t="inlineStr"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="2" t="n">
+        <v>44415.875</v>
+      </c>
+      <c r="B223" t="inlineStr"/>
+      <c r="C223" t="n">
+        <v>38.95941198814373</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="2" t="n">
+        <v>44425.84375</v>
+      </c>
+      <c r="B224" t="n">
+        <v>60.86767051351337</v>
+      </c>
+      <c r="C224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="2" t="n">
+        <v>44425.875</v>
+      </c>
+      <c r="B225" t="inlineStr"/>
+      <c r="C225" t="n">
+        <v>67.84999676587863</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="2" t="n">
+        <v>44430.75</v>
+      </c>
+      <c r="B226" t="n">
+        <v>71.51105413627307</v>
+      </c>
+      <c r="C226" t="inlineStr"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="2" t="n">
+        <v>44430.96875</v>
+      </c>
+      <c r="B227" t="inlineStr"/>
+      <c r="C227" t="n">
+        <v>73.88724202509721</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="2" t="n">
+        <v>44432.65625</v>
+      </c>
+      <c r="B228" t="n">
+        <v>71.76325149451603</v>
+      </c>
+      <c r="C228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="2" t="n">
+        <v>44433.11458333334</v>
+      </c>
+      <c r="B229" t="inlineStr"/>
+      <c r="C229" t="n">
+        <v>71.89387507720097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>